<commit_message>
Modify week5 iteration with user stories for the table
</commit_message>
<xml_diff>
--- a/Project Management/Iteration Planning/Burndown_Charts.xlsx
+++ b/Project Management/Iteration Planning/Burndown_Charts.xlsx
@@ -268,11 +268,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1968272665"/>
-        <c:axId val="1781952315"/>
+        <c:axId val="510238824"/>
+        <c:axId val="780630288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1968272665"/>
+        <c:axId val="510238824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -304,10 +304,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1781952315"/>
+        <c:crossAx val="780630288"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1781952315"/>
+        <c:axId val="780630288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -355,7 +355,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1968272665"/>
+        <c:crossAx val="510238824"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -367,286 +367,6 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600"/>
-            </a:pPr>
-            <a:r>
-              <a:t>Chart title</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4684EE"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 1'!$D$10:$D$11</c:f>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="662307752"/>
-        <c:axId val="531384870"/>
-      </c:barChart>
-      <c:lineChart>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="DC3912"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 1'!$E$10:$E$11</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="FF9900"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 1'!$F$10:$F$11</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="008000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 1'!$G$10:$G$11</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:spPr>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="666666"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 1'!$H$10:$H$11</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:spPr>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="4942CC"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 1'!$I$10:$I$11</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:spPr>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="CB4AC5"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 1'!$J$10:$J$11</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:spPr>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="D6AE00"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 1'!$K$10:$K$11</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="662307752"/>
-        <c:axId val="531384870"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="662307752"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Horizontal axis title</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="531384870"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="531384870"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Left vertical axis title</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt sourceLinked="1" formatCode="General"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47625">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="662307752"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -709,11 +429,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="725346637"/>
-        <c:axId val="126350977"/>
+        <c:axId val="1459837920"/>
+        <c:axId val="368322759"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="725346637"/>
+        <c:axId val="1459837920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,10 +465,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126350977"/>
+        <c:crossAx val="368322759"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126350977"/>
+        <c:axId val="368322759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,7 +516,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="725346637"/>
+        <c:crossAx val="1459837920"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -807,7 +527,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -870,11 +590,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1100496278"/>
-        <c:axId val="1141585406"/>
+        <c:axId val="1751792621"/>
+        <c:axId val="455288618"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1100496278"/>
+        <c:axId val="1751792621"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,10 +626,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1141585406"/>
+        <c:crossAx val="455288618"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1141585406"/>
+        <c:axId val="455288618"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -957,7 +677,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1100496278"/>
+        <c:crossAx val="1751792621"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -968,7 +688,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -1031,11 +751,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="665823456"/>
-        <c:axId val="1521340301"/>
+        <c:axId val="1075488027"/>
+        <c:axId val="1871623954"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="665823456"/>
+        <c:axId val="1075488027"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,10 +787,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1521340301"/>
+        <c:crossAx val="1871623954"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1521340301"/>
+        <c:axId val="1871623954"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +838,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="665823456"/>
+        <c:crossAx val="1075488027"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1129,7 +849,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:plotArea>
@@ -1150,7 +870,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 5'!$D$18:$K$18</c:f>
+              <c:f>'Iteration 5'!$D$21:$K$21</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1170,16 +890,16 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 5'!$D$19:$K$19</c:f>
+              <c:f>'Iteration 5'!$D$22:$K$22</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1825800039"/>
-        <c:axId val="345267841"/>
+        <c:axId val="936251729"/>
+        <c:axId val="125760530"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1825800039"/>
+        <c:axId val="936251729"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1194,10 +914,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345267841"/>
+        <c:crossAx val="125760530"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345267841"/>
+        <c:axId val="125760530"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +948,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1825800039"/>
+        <c:crossAx val="936251729"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1239,7 +959,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -1302,11 +1022,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1735737583"/>
-        <c:axId val="1145949010"/>
+        <c:axId val="596411185"/>
+        <c:axId val="2036974009"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1735737583"/>
+        <c:axId val="596411185"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,10 +1058,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1145949010"/>
+        <c:crossAx val="2036974009"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1145949010"/>
+        <c:axId val="2036974009"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1109,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1735737583"/>
+        <c:crossAx val="596411185"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1422,26 +1142,6 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:absoluteAnchor>
-  <xdr:absoluteAnchor>
-    <xdr:pos y="2057400" x="6591300"/>
-    <xdr:ext cy="3533775" cx="5715000"/>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off y="0" x="0"/>
-        <a:ext cy="0" cx="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1452,7 +1152,7 @@
     <xdr:ext cy="3571875" cx="7620000"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1477,7 +1177,7 @@
     <xdr:ext cy="4333875" cx="9010650"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 4"/>
+        <xdr:cNvPr id="3" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1502,7 +1202,7 @@
     <xdr:ext cy="4105275" cx="8877300"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 5"/>
+        <xdr:cNvPr id="4" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1523,11 +1223,11 @@
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
   <xdr:absoluteAnchor>
-    <xdr:pos y="3810000" x="914400"/>
+    <xdr:pos y="4381500" x="914400"/>
     <xdr:ext cy="4152900" cx="8839200"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 6"/>
+        <xdr:cNvPr id="5" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1552,7 +1252,7 @@
     <xdr:ext cy="4391025" cx="9001125"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 7"/>
+        <xdr:cNvPr id="6" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1982,1006 +1682,6 @@
     <row customHeight="1" r="32" ht="15.0"/>
     <row customHeight="1" r="33" ht="15.0"/>
     <row customHeight="1" r="34" ht="15.0"/>
-    <row customHeight="1" r="35" ht="15.0"/>
-    <row customHeight="1" r="36" ht="15.0"/>
-    <row customHeight="1" r="37" ht="15.0"/>
-    <row customHeight="1" r="38" ht="15.0"/>
-    <row customHeight="1" r="39" ht="15.0"/>
-    <row customHeight="1" r="40" ht="15.0"/>
-    <row customHeight="1" r="41" ht="15.0"/>
-    <row customHeight="1" r="42" ht="15.0"/>
-    <row customHeight="1" r="43" ht="15.0"/>
-    <row customHeight="1" r="44" ht="15.0"/>
-    <row customHeight="1" r="45" ht="15.0"/>
-    <row customHeight="1" r="46" ht="15.0"/>
-    <row customHeight="1" r="47" ht="15.0"/>
-    <row customHeight="1" r="48" ht="15.0"/>
-    <row customHeight="1" r="49" ht="15.0"/>
-    <row customHeight="1" r="50" ht="15.0"/>
-    <row customHeight="1" r="51" ht="15.0"/>
-    <row customHeight="1" r="52" ht="15.0"/>
-    <row customHeight="1" r="53" ht="15.0"/>
-    <row customHeight="1" r="54" ht="15.0"/>
-    <row customHeight="1" r="55" ht="15.0"/>
-    <row customHeight="1" r="56" ht="15.0"/>
-    <row customHeight="1" r="57" ht="15.0"/>
-    <row customHeight="1" r="58" ht="15.0"/>
-    <row customHeight="1" r="59" ht="15.0"/>
-    <row customHeight="1" r="60" ht="15.0"/>
-    <row customHeight="1" r="61" ht="15.0"/>
-    <row customHeight="1" r="62" ht="15.0"/>
-    <row customHeight="1" r="63" ht="15.0"/>
-    <row customHeight="1" r="64" ht="15.0"/>
-    <row customHeight="1" r="65" ht="15.0"/>
-    <row customHeight="1" r="66" ht="15.0"/>
-    <row customHeight="1" r="67" ht="15.0"/>
-    <row customHeight="1" r="68" ht="15.0"/>
-    <row customHeight="1" r="69" ht="15.0"/>
-    <row customHeight="1" r="70" ht="15.0"/>
-    <row customHeight="1" r="71" ht="15.0"/>
-    <row customHeight="1" r="72" ht="15.0"/>
-    <row customHeight="1" r="73" ht="15.0"/>
-    <row customHeight="1" r="74" ht="15.0"/>
-    <row customHeight="1" r="75" ht="15.0"/>
-    <row customHeight="1" r="76" ht="15.0"/>
-    <row customHeight="1" r="77" ht="15.0"/>
-    <row customHeight="1" r="78" ht="15.0"/>
-    <row customHeight="1" r="79" ht="15.0"/>
-    <row customHeight="1" r="80" ht="15.0"/>
-    <row customHeight="1" r="81" ht="15.0"/>
-    <row customHeight="1" r="82" ht="15.0"/>
-    <row customHeight="1" r="83" ht="15.0"/>
-    <row customHeight="1" r="84" ht="15.0"/>
-    <row customHeight="1" r="85" ht="15.0"/>
-    <row customHeight="1" r="86" ht="15.0"/>
-    <row customHeight="1" r="87" ht="15.0"/>
-    <row customHeight="1" r="88" ht="15.0"/>
-    <row customHeight="1" r="89" ht="15.0"/>
-    <row customHeight="1" r="90" ht="15.0"/>
-    <row customHeight="1" r="91" ht="15.0"/>
-    <row customHeight="1" r="92" ht="15.0"/>
-    <row customHeight="1" r="93" ht="15.0"/>
-    <row customHeight="1" r="94" ht="15.0"/>
-    <row customHeight="1" r="95" ht="15.0"/>
-    <row customHeight="1" r="96" ht="15.0"/>
-    <row customHeight="1" r="97" ht="15.0"/>
-    <row customHeight="1" r="98" ht="15.0"/>
-    <row customHeight="1" r="99" ht="15.0"/>
-    <row customHeight="1" r="100" ht="15.0"/>
-    <row customHeight="1" r="101" ht="15.0"/>
-    <row customHeight="1" r="102" ht="15.0"/>
-    <row customHeight="1" r="103" ht="15.0"/>
-    <row customHeight="1" r="104" ht="15.0"/>
-    <row customHeight="1" r="105" ht="15.0"/>
-    <row customHeight="1" r="106" ht="15.0"/>
-    <row customHeight="1" r="107" ht="15.0"/>
-    <row customHeight="1" r="108" ht="15.0"/>
-    <row customHeight="1" r="109" ht="15.0"/>
-    <row customHeight="1" r="110" ht="15.0"/>
-    <row customHeight="1" r="111" ht="15.0"/>
-    <row customHeight="1" r="112" ht="15.0"/>
-    <row customHeight="1" r="113" ht="15.0"/>
-    <row customHeight="1" r="114" ht="15.0"/>
-    <row customHeight="1" r="115" ht="15.0"/>
-    <row customHeight="1" r="116" ht="15.0"/>
-    <row customHeight="1" r="117" ht="15.0"/>
-    <row customHeight="1" r="118" ht="15.0"/>
-    <row customHeight="1" r="119" ht="15.0"/>
-    <row customHeight="1" r="120" ht="15.0"/>
-    <row customHeight="1" r="121" ht="15.0"/>
-    <row customHeight="1" r="122" ht="15.0"/>
-    <row customHeight="1" r="123" ht="15.0"/>
-    <row customHeight="1" r="124" ht="15.0"/>
-    <row customHeight="1" r="125" ht="15.0"/>
-    <row customHeight="1" r="126" ht="15.0"/>
-    <row customHeight="1" r="127" ht="15.0"/>
-    <row customHeight="1" r="128" ht="15.0"/>
-    <row customHeight="1" r="129" ht="15.0"/>
-    <row customHeight="1" r="130" ht="15.0"/>
-    <row customHeight="1" r="131" ht="15.0"/>
-    <row customHeight="1" r="132" ht="15.0"/>
-    <row customHeight="1" r="133" ht="15.0"/>
-    <row customHeight="1" r="134" ht="15.0"/>
-    <row customHeight="1" r="135" ht="15.0"/>
-    <row customHeight="1" r="136" ht="15.0"/>
-    <row customHeight="1" r="137" ht="15.0"/>
-    <row customHeight="1" r="138" ht="15.0"/>
-    <row customHeight="1" r="139" ht="15.0"/>
-    <row customHeight="1" r="140" ht="15.0"/>
-    <row customHeight="1" r="141" ht="15.0"/>
-    <row customHeight="1" r="142" ht="15.0"/>
-    <row customHeight="1" r="143" ht="15.0"/>
-    <row customHeight="1" r="144" ht="15.0"/>
-    <row customHeight="1" r="145" ht="15.0"/>
-    <row customHeight="1" r="146" ht="15.0"/>
-    <row customHeight="1" r="147" ht="15.0"/>
-    <row customHeight="1" r="148" ht="15.0"/>
-    <row customHeight="1" r="149" ht="15.0"/>
-    <row customHeight="1" r="150" ht="15.0"/>
-    <row customHeight="1" r="151" ht="15.0"/>
-    <row customHeight="1" r="152" ht="15.0"/>
-    <row customHeight="1" r="153" ht="15.0"/>
-    <row customHeight="1" r="154" ht="15.0"/>
-    <row customHeight="1" r="155" ht="15.0"/>
-    <row customHeight="1" r="156" ht="15.0"/>
-    <row customHeight="1" r="157" ht="15.0"/>
-    <row customHeight="1" r="158" ht="15.0"/>
-    <row customHeight="1" r="159" ht="15.0"/>
-    <row customHeight="1" r="160" ht="15.0"/>
-    <row customHeight="1" r="161" ht="15.0"/>
-    <row customHeight="1" r="162" ht="15.0"/>
-    <row customHeight="1" r="163" ht="15.0"/>
-    <row customHeight="1" r="164" ht="15.0"/>
-    <row customHeight="1" r="165" ht="15.0"/>
-    <row customHeight="1" r="166" ht="15.0"/>
-    <row customHeight="1" r="167" ht="15.0"/>
-    <row customHeight="1" r="168" ht="15.0"/>
-    <row customHeight="1" r="169" ht="15.0"/>
-    <row customHeight="1" r="170" ht="15.0"/>
-    <row customHeight="1" r="171" ht="15.0"/>
-    <row customHeight="1" r="172" ht="15.0"/>
-    <row customHeight="1" r="173" ht="15.0"/>
-    <row customHeight="1" r="174" ht="15.0"/>
-    <row customHeight="1" r="175" ht="15.0"/>
-    <row customHeight="1" r="176" ht="15.0"/>
-    <row customHeight="1" r="177" ht="15.0"/>
-    <row customHeight="1" r="178" ht="15.0"/>
-    <row customHeight="1" r="179" ht="15.0"/>
-    <row customHeight="1" r="180" ht="15.0"/>
-    <row customHeight="1" r="181" ht="15.0"/>
-    <row customHeight="1" r="182" ht="15.0"/>
-    <row customHeight="1" r="183" ht="15.0"/>
-    <row customHeight="1" r="184" ht="15.0"/>
-    <row customHeight="1" r="185" ht="15.0"/>
-    <row customHeight="1" r="186" ht="15.0"/>
-    <row customHeight="1" r="187" ht="15.0"/>
-    <row customHeight="1" r="188" ht="15.0"/>
-    <row customHeight="1" r="189" ht="15.0"/>
-    <row customHeight="1" r="190" ht="15.0"/>
-    <row customHeight="1" r="191" ht="15.0"/>
-    <row customHeight="1" r="192" ht="15.0"/>
-    <row customHeight="1" r="193" ht="15.0"/>
-    <row customHeight="1" r="194" ht="15.0"/>
-    <row customHeight="1" r="195" ht="15.0"/>
-    <row customHeight="1" r="196" ht="15.0"/>
-    <row customHeight="1" r="197" ht="15.0"/>
-    <row customHeight="1" r="198" ht="15.0"/>
-    <row customHeight="1" r="199" ht="15.0"/>
-    <row customHeight="1" r="200" ht="15.0"/>
-    <row customHeight="1" r="201" ht="15.0"/>
-    <row customHeight="1" r="202" ht="15.0"/>
-    <row customHeight="1" r="203" ht="15.0"/>
-    <row customHeight="1" r="204" ht="15.0"/>
-    <row customHeight="1" r="205" ht="15.0"/>
-    <row customHeight="1" r="206" ht="15.0"/>
-    <row customHeight="1" r="207" ht="15.0"/>
-    <row customHeight="1" r="208" ht="15.0"/>
-    <row customHeight="1" r="209" ht="15.0"/>
-    <row customHeight="1" r="210" ht="15.0"/>
-    <row customHeight="1" r="211" ht="15.0"/>
-    <row customHeight="1" r="212" ht="15.0"/>
-    <row customHeight="1" r="213" ht="15.0"/>
-    <row customHeight="1" r="214" ht="15.0"/>
-    <row customHeight="1" r="215" ht="15.0"/>
-    <row customHeight="1" r="216" ht="15.0"/>
-    <row customHeight="1" r="217" ht="15.0"/>
-    <row customHeight="1" r="218" ht="15.0"/>
-    <row customHeight="1" r="219" ht="15.0"/>
-    <row customHeight="1" r="220" ht="15.0"/>
-    <row customHeight="1" r="221" ht="15.0"/>
-    <row customHeight="1" r="222" ht="15.0"/>
-    <row customHeight="1" r="223" ht="15.0"/>
-    <row customHeight="1" r="224" ht="15.0"/>
-    <row customHeight="1" r="225" ht="15.0"/>
-    <row customHeight="1" r="226" ht="15.0"/>
-    <row customHeight="1" r="227" ht="15.0"/>
-    <row customHeight="1" r="228" ht="15.0"/>
-    <row customHeight="1" r="229" ht="15.0"/>
-    <row customHeight="1" r="230" ht="15.0"/>
-    <row customHeight="1" r="231" ht="15.0"/>
-    <row customHeight="1" r="232" ht="15.0"/>
-    <row customHeight="1" r="233" ht="15.0"/>
-    <row customHeight="1" r="234" ht="15.0"/>
-    <row customHeight="1" r="235" ht="15.0"/>
-    <row customHeight="1" r="236" ht="15.0"/>
-    <row customHeight="1" r="237" ht="15.0"/>
-    <row customHeight="1" r="238" ht="15.0"/>
-    <row customHeight="1" r="239" ht="15.0"/>
-    <row customHeight="1" r="240" ht="15.0"/>
-    <row customHeight="1" r="241" ht="15.0"/>
-    <row customHeight="1" r="242" ht="15.0"/>
-    <row customHeight="1" r="243" ht="15.0"/>
-    <row customHeight="1" r="244" ht="15.0"/>
-    <row customHeight="1" r="245" ht="15.0"/>
-    <row customHeight="1" r="246" ht="15.0"/>
-    <row customHeight="1" r="247" ht="15.0"/>
-    <row customHeight="1" r="248" ht="15.0"/>
-    <row customHeight="1" r="249" ht="15.0"/>
-    <row customHeight="1" r="250" ht="15.0"/>
-    <row customHeight="1" r="251" ht="15.0"/>
-    <row customHeight="1" r="252" ht="15.0"/>
-    <row customHeight="1" r="253" ht="15.0"/>
-    <row customHeight="1" r="254" ht="15.0"/>
-    <row customHeight="1" r="255" ht="15.0"/>
-    <row customHeight="1" r="256" ht="15.0"/>
-    <row customHeight="1" r="257" ht="15.0"/>
-    <row customHeight="1" r="258" ht="15.0"/>
-    <row customHeight="1" r="259" ht="15.0"/>
-    <row customHeight="1" r="260" ht="15.0"/>
-    <row customHeight="1" r="261" ht="15.0"/>
-    <row customHeight="1" r="262" ht="15.0"/>
-    <row customHeight="1" r="263" ht="15.0"/>
-    <row customHeight="1" r="264" ht="15.0"/>
-    <row customHeight="1" r="265" ht="15.0"/>
-    <row customHeight="1" r="266" ht="15.0"/>
-    <row customHeight="1" r="267" ht="15.0"/>
-    <row customHeight="1" r="268" ht="15.0"/>
-    <row customHeight="1" r="269" ht="15.0"/>
-    <row customHeight="1" r="270" ht="15.0"/>
-    <row customHeight="1" r="271" ht="15.0"/>
-    <row customHeight="1" r="272" ht="15.0"/>
-    <row customHeight="1" r="273" ht="15.0"/>
-    <row customHeight="1" r="274" ht="15.0"/>
-    <row customHeight="1" r="275" ht="15.0"/>
-    <row customHeight="1" r="276" ht="15.0"/>
-    <row customHeight="1" r="277" ht="15.0"/>
-    <row customHeight="1" r="278" ht="15.0"/>
-    <row customHeight="1" r="279" ht="15.0"/>
-    <row customHeight="1" r="280" ht="15.0"/>
-    <row customHeight="1" r="281" ht="15.0"/>
-    <row customHeight="1" r="282" ht="15.0"/>
-    <row customHeight="1" r="283" ht="15.0"/>
-    <row customHeight="1" r="284" ht="15.0"/>
-    <row customHeight="1" r="285" ht="15.0"/>
-    <row customHeight="1" r="286" ht="15.0"/>
-    <row customHeight="1" r="287" ht="15.0"/>
-    <row customHeight="1" r="288" ht="15.0"/>
-    <row customHeight="1" r="289" ht="15.0"/>
-    <row customHeight="1" r="290" ht="15.0"/>
-    <row customHeight="1" r="291" ht="15.0"/>
-    <row customHeight="1" r="292" ht="15.0"/>
-    <row customHeight="1" r="293" ht="15.0"/>
-    <row customHeight="1" r="294" ht="15.0"/>
-    <row customHeight="1" r="295" ht="15.0"/>
-    <row customHeight="1" r="296" ht="15.0"/>
-    <row customHeight="1" r="297" ht="15.0"/>
-    <row customHeight="1" r="298" ht="15.0"/>
-    <row customHeight="1" r="299" ht="15.0"/>
-    <row customHeight="1" r="300" ht="15.0"/>
-    <row customHeight="1" r="301" ht="15.0"/>
-    <row customHeight="1" r="302" ht="15.0"/>
-    <row customHeight="1" r="303" ht="15.0"/>
-    <row customHeight="1" r="304" ht="15.0"/>
-    <row customHeight="1" r="305" ht="15.0"/>
-    <row customHeight="1" r="306" ht="15.0"/>
-    <row customHeight="1" r="307" ht="15.0"/>
-    <row customHeight="1" r="308" ht="15.0"/>
-    <row customHeight="1" r="309" ht="15.0"/>
-    <row customHeight="1" r="310" ht="15.0"/>
-    <row customHeight="1" r="311" ht="15.0"/>
-    <row customHeight="1" r="312" ht="15.0"/>
-    <row customHeight="1" r="313" ht="15.0"/>
-    <row customHeight="1" r="314" ht="15.0"/>
-    <row customHeight="1" r="315" ht="15.0"/>
-    <row customHeight="1" r="316" ht="15.0"/>
-    <row customHeight="1" r="317" ht="15.0"/>
-    <row customHeight="1" r="318" ht="15.0"/>
-    <row customHeight="1" r="319" ht="15.0"/>
-    <row customHeight="1" r="320" ht="15.0"/>
-    <row customHeight="1" r="321" ht="15.0"/>
-    <row customHeight="1" r="322" ht="15.0"/>
-    <row customHeight="1" r="323" ht="15.0"/>
-    <row customHeight="1" r="324" ht="15.0"/>
-    <row customHeight="1" r="325" ht="15.0"/>
-    <row customHeight="1" r="326" ht="15.0"/>
-    <row customHeight="1" r="327" ht="15.0"/>
-    <row customHeight="1" r="328" ht="15.0"/>
-    <row customHeight="1" r="329" ht="15.0"/>
-    <row customHeight="1" r="330" ht="15.0"/>
-    <row customHeight="1" r="331" ht="15.0"/>
-    <row customHeight="1" r="332" ht="15.0"/>
-    <row customHeight="1" r="333" ht="15.0"/>
-    <row customHeight="1" r="334" ht="15.0"/>
-    <row customHeight="1" r="335" ht="15.0"/>
-    <row customHeight="1" r="336" ht="15.0"/>
-    <row customHeight="1" r="337" ht="15.0"/>
-    <row customHeight="1" r="338" ht="15.0"/>
-    <row customHeight="1" r="339" ht="15.0"/>
-    <row customHeight="1" r="340" ht="15.0"/>
-    <row customHeight="1" r="341" ht="15.0"/>
-    <row customHeight="1" r="342" ht="15.0"/>
-    <row customHeight="1" r="343" ht="15.0"/>
-    <row customHeight="1" r="344" ht="15.0"/>
-    <row customHeight="1" r="345" ht="15.0"/>
-    <row customHeight="1" r="346" ht="15.0"/>
-    <row customHeight="1" r="347" ht="15.0"/>
-    <row customHeight="1" r="348" ht="15.0"/>
-    <row customHeight="1" r="349" ht="15.0"/>
-    <row customHeight="1" r="350" ht="15.0"/>
-    <row customHeight="1" r="351" ht="15.0"/>
-    <row customHeight="1" r="352" ht="15.0"/>
-    <row customHeight="1" r="353" ht="15.0"/>
-    <row customHeight="1" r="354" ht="15.0"/>
-    <row customHeight="1" r="355" ht="15.0"/>
-    <row customHeight="1" r="356" ht="15.0"/>
-    <row customHeight="1" r="357" ht="15.0"/>
-    <row customHeight="1" r="358" ht="15.0"/>
-    <row customHeight="1" r="359" ht="15.0"/>
-    <row customHeight="1" r="360" ht="15.0"/>
-    <row customHeight="1" r="361" ht="15.0"/>
-    <row customHeight="1" r="362" ht="15.0"/>
-    <row customHeight="1" r="363" ht="15.0"/>
-    <row customHeight="1" r="364" ht="15.0"/>
-    <row customHeight="1" r="365" ht="15.0"/>
-    <row customHeight="1" r="366" ht="15.0"/>
-    <row customHeight="1" r="367" ht="15.0"/>
-    <row customHeight="1" r="368" ht="15.0"/>
-    <row customHeight="1" r="369" ht="15.0"/>
-    <row customHeight="1" r="370" ht="15.0"/>
-    <row customHeight="1" r="371" ht="15.0"/>
-    <row customHeight="1" r="372" ht="15.0"/>
-    <row customHeight="1" r="373" ht="15.0"/>
-    <row customHeight="1" r="374" ht="15.0"/>
-    <row customHeight="1" r="375" ht="15.0"/>
-    <row customHeight="1" r="376" ht="15.0"/>
-    <row customHeight="1" r="377" ht="15.0"/>
-    <row customHeight="1" r="378" ht="15.0"/>
-    <row customHeight="1" r="379" ht="15.0"/>
-    <row customHeight="1" r="380" ht="15.0"/>
-    <row customHeight="1" r="381" ht="15.0"/>
-    <row customHeight="1" r="382" ht="15.0"/>
-    <row customHeight="1" r="383" ht="15.0"/>
-    <row customHeight="1" r="384" ht="15.0"/>
-    <row customHeight="1" r="385" ht="15.0"/>
-    <row customHeight="1" r="386" ht="15.0"/>
-    <row customHeight="1" r="387" ht="15.0"/>
-    <row customHeight="1" r="388" ht="15.0"/>
-    <row customHeight="1" r="389" ht="15.0"/>
-    <row customHeight="1" r="390" ht="15.0"/>
-    <row customHeight="1" r="391" ht="15.0"/>
-    <row customHeight="1" r="392" ht="15.0"/>
-    <row customHeight="1" r="393" ht="15.0"/>
-    <row customHeight="1" r="394" ht="15.0"/>
-    <row customHeight="1" r="395" ht="15.0"/>
-    <row customHeight="1" r="396" ht="15.0"/>
-    <row customHeight="1" r="397" ht="15.0"/>
-    <row customHeight="1" r="398" ht="15.0"/>
-    <row customHeight="1" r="399" ht="15.0"/>
-    <row customHeight="1" r="400" ht="15.0"/>
-    <row customHeight="1" r="401" ht="15.0"/>
-    <row customHeight="1" r="402" ht="15.0"/>
-    <row customHeight="1" r="403" ht="15.0"/>
-    <row customHeight="1" r="404" ht="15.0"/>
-    <row customHeight="1" r="405" ht="15.0"/>
-    <row customHeight="1" r="406" ht="15.0"/>
-    <row customHeight="1" r="407" ht="15.0"/>
-    <row customHeight="1" r="408" ht="15.0"/>
-    <row customHeight="1" r="409" ht="15.0"/>
-    <row customHeight="1" r="410" ht="15.0"/>
-    <row customHeight="1" r="411" ht="15.0"/>
-    <row customHeight="1" r="412" ht="15.0"/>
-    <row customHeight="1" r="413" ht="15.0"/>
-    <row customHeight="1" r="414" ht="15.0"/>
-    <row customHeight="1" r="415" ht="15.0"/>
-    <row customHeight="1" r="416" ht="15.0"/>
-    <row customHeight="1" r="417" ht="15.0"/>
-    <row customHeight="1" r="418" ht="15.0"/>
-    <row customHeight="1" r="419" ht="15.0"/>
-    <row customHeight="1" r="420" ht="15.0"/>
-    <row customHeight="1" r="421" ht="15.0"/>
-    <row customHeight="1" r="422" ht="15.0"/>
-    <row customHeight="1" r="423" ht="15.0"/>
-    <row customHeight="1" r="424" ht="15.0"/>
-    <row customHeight="1" r="425" ht="15.0"/>
-    <row customHeight="1" r="426" ht="15.0"/>
-    <row customHeight="1" r="427" ht="15.0"/>
-    <row customHeight="1" r="428" ht="15.0"/>
-    <row customHeight="1" r="429" ht="15.0"/>
-    <row customHeight="1" r="430" ht="15.0"/>
-    <row customHeight="1" r="431" ht="15.0"/>
-    <row customHeight="1" r="432" ht="15.0"/>
-    <row customHeight="1" r="433" ht="15.0"/>
-    <row customHeight="1" r="434" ht="15.0"/>
-    <row customHeight="1" r="435" ht="15.0"/>
-    <row customHeight="1" r="436" ht="15.0"/>
-    <row customHeight="1" r="437" ht="15.0"/>
-    <row customHeight="1" r="438" ht="15.0"/>
-    <row customHeight="1" r="439" ht="15.0"/>
-    <row customHeight="1" r="440" ht="15.0"/>
-    <row customHeight="1" r="441" ht="15.0"/>
-    <row customHeight="1" r="442" ht="15.0"/>
-    <row customHeight="1" r="443" ht="15.0"/>
-    <row customHeight="1" r="444" ht="15.0"/>
-    <row customHeight="1" r="445" ht="15.0"/>
-    <row customHeight="1" r="446" ht="15.0"/>
-    <row customHeight="1" r="447" ht="15.0"/>
-    <row customHeight="1" r="448" ht="15.0"/>
-    <row customHeight="1" r="449" ht="15.0"/>
-    <row customHeight="1" r="450" ht="15.0"/>
-    <row customHeight="1" r="451" ht="15.0"/>
-    <row customHeight="1" r="452" ht="15.0"/>
-    <row customHeight="1" r="453" ht="15.0"/>
-    <row customHeight="1" r="454" ht="15.0"/>
-    <row customHeight="1" r="455" ht="15.0"/>
-    <row customHeight="1" r="456" ht="15.0"/>
-    <row customHeight="1" r="457" ht="15.0"/>
-    <row customHeight="1" r="458" ht="15.0"/>
-    <row customHeight="1" r="459" ht="15.0"/>
-    <row customHeight="1" r="460" ht="15.0"/>
-    <row customHeight="1" r="461" ht="15.0"/>
-    <row customHeight="1" r="462" ht="15.0"/>
-    <row customHeight="1" r="463" ht="15.0"/>
-    <row customHeight="1" r="464" ht="15.0"/>
-    <row customHeight="1" r="465" ht="15.0"/>
-    <row customHeight="1" r="466" ht="15.0"/>
-    <row customHeight="1" r="467" ht="15.0"/>
-    <row customHeight="1" r="468" ht="15.0"/>
-    <row customHeight="1" r="469" ht="15.0"/>
-    <row customHeight="1" r="470" ht="15.0"/>
-    <row customHeight="1" r="471" ht="15.0"/>
-    <row customHeight="1" r="472" ht="15.0"/>
-    <row customHeight="1" r="473" ht="15.0"/>
-    <row customHeight="1" r="474" ht="15.0"/>
-    <row customHeight="1" r="475" ht="15.0"/>
-    <row customHeight="1" r="476" ht="15.0"/>
-    <row customHeight="1" r="477" ht="15.0"/>
-    <row customHeight="1" r="478" ht="15.0"/>
-    <row customHeight="1" r="479" ht="15.0"/>
-    <row customHeight="1" r="480" ht="15.0"/>
-    <row customHeight="1" r="481" ht="15.0"/>
-    <row customHeight="1" r="482" ht="15.0"/>
-    <row customHeight="1" r="483" ht="15.0"/>
-    <row customHeight="1" r="484" ht="15.0"/>
-    <row customHeight="1" r="485" ht="15.0"/>
-    <row customHeight="1" r="486" ht="15.0"/>
-    <row customHeight="1" r="487" ht="15.0"/>
-    <row customHeight="1" r="488" ht="15.0"/>
-    <row customHeight="1" r="489" ht="15.0"/>
-    <row customHeight="1" r="490" ht="15.0"/>
-    <row customHeight="1" r="491" ht="15.0"/>
-    <row customHeight="1" r="492" ht="15.0"/>
-    <row customHeight="1" r="493" ht="15.0"/>
-    <row customHeight="1" r="494" ht="15.0"/>
-    <row customHeight="1" r="495" ht="15.0"/>
-    <row customHeight="1" r="496" ht="15.0"/>
-    <row customHeight="1" r="497" ht="15.0"/>
-    <row customHeight="1" r="498" ht="15.0"/>
-    <row customHeight="1" r="499" ht="15.0"/>
-    <row customHeight="1" r="500" ht="15.0"/>
-    <row customHeight="1" r="501" ht="15.0"/>
-    <row customHeight="1" r="502" ht="15.0"/>
-    <row customHeight="1" r="503" ht="15.0"/>
-    <row customHeight="1" r="504" ht="15.0"/>
-    <row customHeight="1" r="505" ht="15.0"/>
-    <row customHeight="1" r="506" ht="15.0"/>
-    <row customHeight="1" r="507" ht="15.0"/>
-    <row customHeight="1" r="508" ht="15.0"/>
-    <row customHeight="1" r="509" ht="15.0"/>
-    <row customHeight="1" r="510" ht="15.0"/>
-    <row customHeight="1" r="511" ht="15.0"/>
-    <row customHeight="1" r="512" ht="15.0"/>
-    <row customHeight="1" r="513" ht="15.0"/>
-    <row customHeight="1" r="514" ht="15.0"/>
-    <row customHeight="1" r="515" ht="15.0"/>
-    <row customHeight="1" r="516" ht="15.0"/>
-    <row customHeight="1" r="517" ht="15.0"/>
-    <row customHeight="1" r="518" ht="15.0"/>
-    <row customHeight="1" r="519" ht="15.0"/>
-    <row customHeight="1" r="520" ht="15.0"/>
-    <row customHeight="1" r="521" ht="15.0"/>
-    <row customHeight="1" r="522" ht="15.0"/>
-    <row customHeight="1" r="523" ht="15.0"/>
-    <row customHeight="1" r="524" ht="15.0"/>
-    <row customHeight="1" r="525" ht="15.0"/>
-    <row customHeight="1" r="526" ht="15.0"/>
-    <row customHeight="1" r="527" ht="15.0"/>
-    <row customHeight="1" r="528" ht="15.0"/>
-    <row customHeight="1" r="529" ht="15.0"/>
-    <row customHeight="1" r="530" ht="15.0"/>
-    <row customHeight="1" r="531" ht="15.0"/>
-    <row customHeight="1" r="532" ht="15.0"/>
-    <row customHeight="1" r="533" ht="15.0"/>
-    <row customHeight="1" r="534" ht="15.0"/>
-    <row customHeight="1" r="535" ht="15.0"/>
-    <row customHeight="1" r="536" ht="15.0"/>
-    <row customHeight="1" r="537" ht="15.0"/>
-    <row customHeight="1" r="538" ht="15.0"/>
-    <row customHeight="1" r="539" ht="15.0"/>
-    <row customHeight="1" r="540" ht="15.0"/>
-    <row customHeight="1" r="541" ht="15.0"/>
-    <row customHeight="1" r="542" ht="15.0"/>
-    <row customHeight="1" r="543" ht="15.0"/>
-    <row customHeight="1" r="544" ht="15.0"/>
-    <row customHeight="1" r="545" ht="15.0"/>
-    <row customHeight="1" r="546" ht="15.0"/>
-    <row customHeight="1" r="547" ht="15.0"/>
-    <row customHeight="1" r="548" ht="15.0"/>
-    <row customHeight="1" r="549" ht="15.0"/>
-    <row customHeight="1" r="550" ht="15.0"/>
-    <row customHeight="1" r="551" ht="15.0"/>
-    <row customHeight="1" r="552" ht="15.0"/>
-    <row customHeight="1" r="553" ht="15.0"/>
-    <row customHeight="1" r="554" ht="15.0"/>
-    <row customHeight="1" r="555" ht="15.0"/>
-    <row customHeight="1" r="556" ht="15.0"/>
-    <row customHeight="1" r="557" ht="15.0"/>
-    <row customHeight="1" r="558" ht="15.0"/>
-    <row customHeight="1" r="559" ht="15.0"/>
-    <row customHeight="1" r="560" ht="15.0"/>
-    <row customHeight="1" r="561" ht="15.0"/>
-    <row customHeight="1" r="562" ht="15.0"/>
-    <row customHeight="1" r="563" ht="15.0"/>
-    <row customHeight="1" r="564" ht="15.0"/>
-    <row customHeight="1" r="565" ht="15.0"/>
-    <row customHeight="1" r="566" ht="15.0"/>
-    <row customHeight="1" r="567" ht="15.0"/>
-    <row customHeight="1" r="568" ht="15.0"/>
-    <row customHeight="1" r="569" ht="15.0"/>
-    <row customHeight="1" r="570" ht="15.0"/>
-    <row customHeight="1" r="571" ht="15.0"/>
-    <row customHeight="1" r="572" ht="15.0"/>
-    <row customHeight="1" r="573" ht="15.0"/>
-    <row customHeight="1" r="574" ht="15.0"/>
-    <row customHeight="1" r="575" ht="15.0"/>
-    <row customHeight="1" r="576" ht="15.0"/>
-    <row customHeight="1" r="577" ht="15.0"/>
-    <row customHeight="1" r="578" ht="15.0"/>
-    <row customHeight="1" r="579" ht="15.0"/>
-    <row customHeight="1" r="580" ht="15.0"/>
-    <row customHeight="1" r="581" ht="15.0"/>
-    <row customHeight="1" r="582" ht="15.0"/>
-    <row customHeight="1" r="583" ht="15.0"/>
-    <row customHeight="1" r="584" ht="15.0"/>
-    <row customHeight="1" r="585" ht="15.0"/>
-    <row customHeight="1" r="586" ht="15.0"/>
-    <row customHeight="1" r="587" ht="15.0"/>
-    <row customHeight="1" r="588" ht="15.0"/>
-    <row customHeight="1" r="589" ht="15.0"/>
-    <row customHeight="1" r="590" ht="15.0"/>
-    <row customHeight="1" r="591" ht="15.0"/>
-    <row customHeight="1" r="592" ht="15.0"/>
-    <row customHeight="1" r="593" ht="15.0"/>
-    <row customHeight="1" r="594" ht="15.0"/>
-    <row customHeight="1" r="595" ht="15.0"/>
-    <row customHeight="1" r="596" ht="15.0"/>
-    <row customHeight="1" r="597" ht="15.0"/>
-    <row customHeight="1" r="598" ht="15.0"/>
-    <row customHeight="1" r="599" ht="15.0"/>
-    <row customHeight="1" r="600" ht="15.0"/>
-    <row customHeight="1" r="601" ht="15.0"/>
-    <row customHeight="1" r="602" ht="15.0"/>
-    <row customHeight="1" r="603" ht="15.0"/>
-    <row customHeight="1" r="604" ht="15.0"/>
-    <row customHeight="1" r="605" ht="15.0"/>
-    <row customHeight="1" r="606" ht="15.0"/>
-    <row customHeight="1" r="607" ht="15.0"/>
-    <row customHeight="1" r="608" ht="15.0"/>
-    <row customHeight="1" r="609" ht="15.0"/>
-    <row customHeight="1" r="610" ht="15.0"/>
-    <row customHeight="1" r="611" ht="15.0"/>
-    <row customHeight="1" r="612" ht="15.0"/>
-    <row customHeight="1" r="613" ht="15.0"/>
-    <row customHeight="1" r="614" ht="15.0"/>
-    <row customHeight="1" r="615" ht="15.0"/>
-    <row customHeight="1" r="616" ht="15.0"/>
-    <row customHeight="1" r="617" ht="15.0"/>
-    <row customHeight="1" r="618" ht="15.0"/>
-    <row customHeight="1" r="619" ht="15.0"/>
-    <row customHeight="1" r="620" ht="15.0"/>
-    <row customHeight="1" r="621" ht="15.0"/>
-    <row customHeight="1" r="622" ht="15.0"/>
-    <row customHeight="1" r="623" ht="15.0"/>
-    <row customHeight="1" r="624" ht="15.0"/>
-    <row customHeight="1" r="625" ht="15.0"/>
-    <row customHeight="1" r="626" ht="15.0"/>
-    <row customHeight="1" r="627" ht="15.0"/>
-    <row customHeight="1" r="628" ht="15.0"/>
-    <row customHeight="1" r="629" ht="15.0"/>
-    <row customHeight="1" r="630" ht="15.0"/>
-    <row customHeight="1" r="631" ht="15.0"/>
-    <row customHeight="1" r="632" ht="15.0"/>
-    <row customHeight="1" r="633" ht="15.0"/>
-    <row customHeight="1" r="634" ht="15.0"/>
-    <row customHeight="1" r="635" ht="15.0"/>
-    <row customHeight="1" r="636" ht="15.0"/>
-    <row customHeight="1" r="637" ht="15.0"/>
-    <row customHeight="1" r="638" ht="15.0"/>
-    <row customHeight="1" r="639" ht="15.0"/>
-    <row customHeight="1" r="640" ht="15.0"/>
-    <row customHeight="1" r="641" ht="15.0"/>
-    <row customHeight="1" r="642" ht="15.0"/>
-    <row customHeight="1" r="643" ht="15.0"/>
-    <row customHeight="1" r="644" ht="15.0"/>
-    <row customHeight="1" r="645" ht="15.0"/>
-    <row customHeight="1" r="646" ht="15.0"/>
-    <row customHeight="1" r="647" ht="15.0"/>
-    <row customHeight="1" r="648" ht="15.0"/>
-    <row customHeight="1" r="649" ht="15.0"/>
-    <row customHeight="1" r="650" ht="15.0"/>
-    <row customHeight="1" r="651" ht="15.0"/>
-    <row customHeight="1" r="652" ht="15.0"/>
-    <row customHeight="1" r="653" ht="15.0"/>
-    <row customHeight="1" r="654" ht="15.0"/>
-    <row customHeight="1" r="655" ht="15.0"/>
-    <row customHeight="1" r="656" ht="15.0"/>
-    <row customHeight="1" r="657" ht="15.0"/>
-    <row customHeight="1" r="658" ht="15.0"/>
-    <row customHeight="1" r="659" ht="15.0"/>
-    <row customHeight="1" r="660" ht="15.0"/>
-    <row customHeight="1" r="661" ht="15.0"/>
-    <row customHeight="1" r="662" ht="15.0"/>
-    <row customHeight="1" r="663" ht="15.0"/>
-    <row customHeight="1" r="664" ht="15.0"/>
-    <row customHeight="1" r="665" ht="15.0"/>
-    <row customHeight="1" r="666" ht="15.0"/>
-    <row customHeight="1" r="667" ht="15.0"/>
-    <row customHeight="1" r="668" ht="15.0"/>
-    <row customHeight="1" r="669" ht="15.0"/>
-    <row customHeight="1" r="670" ht="15.0"/>
-    <row customHeight="1" r="671" ht="15.0"/>
-    <row customHeight="1" r="672" ht="15.0"/>
-    <row customHeight="1" r="673" ht="15.0"/>
-    <row customHeight="1" r="674" ht="15.0"/>
-    <row customHeight="1" r="675" ht="15.0"/>
-    <row customHeight="1" r="676" ht="15.0"/>
-    <row customHeight="1" r="677" ht="15.0"/>
-    <row customHeight="1" r="678" ht="15.0"/>
-    <row customHeight="1" r="679" ht="15.0"/>
-    <row customHeight="1" r="680" ht="15.0"/>
-    <row customHeight="1" r="681" ht="15.0"/>
-    <row customHeight="1" r="682" ht="15.0"/>
-    <row customHeight="1" r="683" ht="15.0"/>
-    <row customHeight="1" r="684" ht="15.0"/>
-    <row customHeight="1" r="685" ht="15.0"/>
-    <row customHeight="1" r="686" ht="15.0"/>
-    <row customHeight="1" r="687" ht="15.0"/>
-    <row customHeight="1" r="688" ht="15.0"/>
-    <row customHeight="1" r="689" ht="15.0"/>
-    <row customHeight="1" r="690" ht="15.0"/>
-    <row customHeight="1" r="691" ht="15.0"/>
-    <row customHeight="1" r="692" ht="15.0"/>
-    <row customHeight="1" r="693" ht="15.0"/>
-    <row customHeight="1" r="694" ht="15.0"/>
-    <row customHeight="1" r="695" ht="15.0"/>
-    <row customHeight="1" r="696" ht="15.0"/>
-    <row customHeight="1" r="697" ht="15.0"/>
-    <row customHeight="1" r="698" ht="15.0"/>
-    <row customHeight="1" r="699" ht="15.0"/>
-    <row customHeight="1" r="700" ht="15.0"/>
-    <row customHeight="1" r="701" ht="15.0"/>
-    <row customHeight="1" r="702" ht="15.0"/>
-    <row customHeight="1" r="703" ht="15.0"/>
-    <row customHeight="1" r="704" ht="15.0"/>
-    <row customHeight="1" r="705" ht="15.0"/>
-    <row customHeight="1" r="706" ht="15.0"/>
-    <row customHeight="1" r="707" ht="15.0"/>
-    <row customHeight="1" r="708" ht="15.0"/>
-    <row customHeight="1" r="709" ht="15.0"/>
-    <row customHeight="1" r="710" ht="15.0"/>
-    <row customHeight="1" r="711" ht="15.0"/>
-    <row customHeight="1" r="712" ht="15.0"/>
-    <row customHeight="1" r="713" ht="15.0"/>
-    <row customHeight="1" r="714" ht="15.0"/>
-    <row customHeight="1" r="715" ht="15.0"/>
-    <row customHeight="1" r="716" ht="15.0"/>
-    <row customHeight="1" r="717" ht="15.0"/>
-    <row customHeight="1" r="718" ht="15.0"/>
-    <row customHeight="1" r="719" ht="15.0"/>
-    <row customHeight="1" r="720" ht="15.0"/>
-    <row customHeight="1" r="721" ht="15.0"/>
-    <row customHeight="1" r="722" ht="15.0"/>
-    <row customHeight="1" r="723" ht="15.0"/>
-    <row customHeight="1" r="724" ht="15.0"/>
-    <row customHeight="1" r="725" ht="15.0"/>
-    <row customHeight="1" r="726" ht="15.0"/>
-    <row customHeight="1" r="727" ht="15.0"/>
-    <row customHeight="1" r="728" ht="15.0"/>
-    <row customHeight="1" r="729" ht="15.0"/>
-    <row customHeight="1" r="730" ht="15.0"/>
-    <row customHeight="1" r="731" ht="15.0"/>
-    <row customHeight="1" r="732" ht="15.0"/>
-    <row customHeight="1" r="733" ht="15.0"/>
-    <row customHeight="1" r="734" ht="15.0"/>
-    <row customHeight="1" r="735" ht="15.0"/>
-    <row customHeight="1" r="736" ht="15.0"/>
-    <row customHeight="1" r="737" ht="15.0"/>
-    <row customHeight="1" r="738" ht="15.0"/>
-    <row customHeight="1" r="739" ht="15.0"/>
-    <row customHeight="1" r="740" ht="15.0"/>
-    <row customHeight="1" r="741" ht="15.0"/>
-    <row customHeight="1" r="742" ht="15.0"/>
-    <row customHeight="1" r="743" ht="15.0"/>
-    <row customHeight="1" r="744" ht="15.0"/>
-    <row customHeight="1" r="745" ht="15.0"/>
-    <row customHeight="1" r="746" ht="15.0"/>
-    <row customHeight="1" r="747" ht="15.0"/>
-    <row customHeight="1" r="748" ht="15.0"/>
-    <row customHeight="1" r="749" ht="15.0"/>
-    <row customHeight="1" r="750" ht="15.0"/>
-    <row customHeight="1" r="751" ht="15.0"/>
-    <row customHeight="1" r="752" ht="15.0"/>
-    <row customHeight="1" r="753" ht="15.0"/>
-    <row customHeight="1" r="754" ht="15.0"/>
-    <row customHeight="1" r="755" ht="15.0"/>
-    <row customHeight="1" r="756" ht="15.0"/>
-    <row customHeight="1" r="757" ht="15.0"/>
-    <row customHeight="1" r="758" ht="15.0"/>
-    <row customHeight="1" r="759" ht="15.0"/>
-    <row customHeight="1" r="760" ht="15.0"/>
-    <row customHeight="1" r="761" ht="15.0"/>
-    <row customHeight="1" r="762" ht="15.0"/>
-    <row customHeight="1" r="763" ht="15.0"/>
-    <row customHeight="1" r="764" ht="15.0"/>
-    <row customHeight="1" r="765" ht="15.0"/>
-    <row customHeight="1" r="766" ht="15.0"/>
-    <row customHeight="1" r="767" ht="15.0"/>
-    <row customHeight="1" r="768" ht="15.0"/>
-    <row customHeight="1" r="769" ht="15.0"/>
-    <row customHeight="1" r="770" ht="15.0"/>
-    <row customHeight="1" r="771" ht="15.0"/>
-    <row customHeight="1" r="772" ht="15.0"/>
-    <row customHeight="1" r="773" ht="15.0"/>
-    <row customHeight="1" r="774" ht="15.0"/>
-    <row customHeight="1" r="775" ht="15.0"/>
-    <row customHeight="1" r="776" ht="15.0"/>
-    <row customHeight="1" r="777" ht="15.0"/>
-    <row customHeight="1" r="778" ht="15.0"/>
-    <row customHeight="1" r="779" ht="15.0"/>
-    <row customHeight="1" r="780" ht="15.0"/>
-    <row customHeight="1" r="781" ht="15.0"/>
-    <row customHeight="1" r="782" ht="15.0"/>
-    <row customHeight="1" r="783" ht="15.0"/>
-    <row customHeight="1" r="784" ht="15.0"/>
-    <row customHeight="1" r="785" ht="15.0"/>
-    <row customHeight="1" r="786" ht="15.0"/>
-    <row customHeight="1" r="787" ht="15.0"/>
-    <row customHeight="1" r="788" ht="15.0"/>
-    <row customHeight="1" r="789" ht="15.0"/>
-    <row customHeight="1" r="790" ht="15.0"/>
-    <row customHeight="1" r="791" ht="15.0"/>
-    <row customHeight="1" r="792" ht="15.0"/>
-    <row customHeight="1" r="793" ht="15.0"/>
-    <row customHeight="1" r="794" ht="15.0"/>
-    <row customHeight="1" r="795" ht="15.0"/>
-    <row customHeight="1" r="796" ht="15.0"/>
-    <row customHeight="1" r="797" ht="15.0"/>
-    <row customHeight="1" r="798" ht="15.0"/>
-    <row customHeight="1" r="799" ht="15.0"/>
-    <row customHeight="1" r="800" ht="15.0"/>
-    <row customHeight="1" r="801" ht="15.0"/>
-    <row customHeight="1" r="802" ht="15.0"/>
-    <row customHeight="1" r="803" ht="15.0"/>
-    <row customHeight="1" r="804" ht="15.0"/>
-    <row customHeight="1" r="805" ht="15.0"/>
-    <row customHeight="1" r="806" ht="15.0"/>
-    <row customHeight="1" r="807" ht="15.0"/>
-    <row customHeight="1" r="808" ht="15.0"/>
-    <row customHeight="1" r="809" ht="15.0"/>
-    <row customHeight="1" r="810" ht="15.0"/>
-    <row customHeight="1" r="811" ht="15.0"/>
-    <row customHeight="1" r="812" ht="15.0"/>
-    <row customHeight="1" r="813" ht="15.0"/>
-    <row customHeight="1" r="814" ht="15.0"/>
-    <row customHeight="1" r="815" ht="15.0"/>
-    <row customHeight="1" r="816" ht="15.0"/>
-    <row customHeight="1" r="817" ht="15.0"/>
-    <row customHeight="1" r="818" ht="15.0"/>
-    <row customHeight="1" r="819" ht="15.0"/>
-    <row customHeight="1" r="820" ht="15.0"/>
-    <row customHeight="1" r="821" ht="15.0"/>
-    <row customHeight="1" r="822" ht="15.0"/>
-    <row customHeight="1" r="823" ht="15.0"/>
-    <row customHeight="1" r="824" ht="15.0"/>
-    <row customHeight="1" r="825" ht="15.0"/>
-    <row customHeight="1" r="826" ht="15.0"/>
-    <row customHeight="1" r="827" ht="15.0"/>
-    <row customHeight="1" r="828" ht="15.0"/>
-    <row customHeight="1" r="829" ht="15.0"/>
-    <row customHeight="1" r="830" ht="15.0"/>
-    <row customHeight="1" r="831" ht="15.0"/>
-    <row customHeight="1" r="832" ht="15.0"/>
-    <row customHeight="1" r="833" ht="15.0"/>
-    <row customHeight="1" r="834" ht="15.0"/>
-    <row customHeight="1" r="835" ht="15.0"/>
-    <row customHeight="1" r="836" ht="15.0"/>
-    <row customHeight="1" r="837" ht="15.0"/>
-    <row customHeight="1" r="838" ht="15.0"/>
-    <row customHeight="1" r="839" ht="15.0"/>
-    <row customHeight="1" r="840" ht="15.0"/>
-    <row customHeight="1" r="841" ht="15.0"/>
-    <row customHeight="1" r="842" ht="15.0"/>
-    <row customHeight="1" r="843" ht="15.0"/>
-    <row customHeight="1" r="844" ht="15.0"/>
-    <row customHeight="1" r="845" ht="15.0"/>
-    <row customHeight="1" r="846" ht="15.0"/>
-    <row customHeight="1" r="847" ht="15.0"/>
-    <row customHeight="1" r="848" ht="15.0"/>
-    <row customHeight="1" r="849" ht="15.0"/>
-    <row customHeight="1" r="850" ht="15.0"/>
-    <row customHeight="1" r="851" ht="15.0"/>
-    <row customHeight="1" r="852" ht="15.0"/>
-    <row customHeight="1" r="853" ht="15.0"/>
-    <row customHeight="1" r="854" ht="15.0"/>
-    <row customHeight="1" r="855" ht="15.0"/>
-    <row customHeight="1" r="856" ht="15.0"/>
-    <row customHeight="1" r="857" ht="15.0"/>
-    <row customHeight="1" r="858" ht="15.0"/>
-    <row customHeight="1" r="859" ht="15.0"/>
-    <row customHeight="1" r="860" ht="15.0"/>
-    <row customHeight="1" r="861" ht="15.0"/>
-    <row customHeight="1" r="862" ht="15.0"/>
-    <row customHeight="1" r="863" ht="15.0"/>
-    <row customHeight="1" r="864" ht="15.0"/>
-    <row customHeight="1" r="865" ht="15.0"/>
-    <row customHeight="1" r="866" ht="15.0"/>
-    <row customHeight="1" r="867" ht="15.0"/>
-    <row customHeight="1" r="868" ht="15.0"/>
-    <row customHeight="1" r="869" ht="15.0"/>
-    <row customHeight="1" r="870" ht="15.0"/>
-    <row customHeight="1" r="871" ht="15.0"/>
-    <row customHeight="1" r="872" ht="15.0"/>
-    <row customHeight="1" r="873" ht="15.0"/>
-    <row customHeight="1" r="874" ht="15.0"/>
-    <row customHeight="1" r="875" ht="15.0"/>
-    <row customHeight="1" r="876" ht="15.0"/>
-    <row customHeight="1" r="877" ht="15.0"/>
-    <row customHeight="1" r="878" ht="15.0"/>
-    <row customHeight="1" r="879" ht="15.0"/>
-    <row customHeight="1" r="880" ht="15.0"/>
-    <row customHeight="1" r="881" ht="15.0"/>
-    <row customHeight="1" r="882" ht="15.0"/>
-    <row customHeight="1" r="883" ht="15.0"/>
-    <row customHeight="1" r="884" ht="15.0"/>
-    <row customHeight="1" r="885" ht="15.0"/>
-    <row customHeight="1" r="886" ht="15.0"/>
-    <row customHeight="1" r="887" ht="15.0"/>
-    <row customHeight="1" r="888" ht="15.0"/>
-    <row customHeight="1" r="889" ht="15.0"/>
-    <row customHeight="1" r="890" ht="15.0"/>
-    <row customHeight="1" r="891" ht="15.0"/>
-    <row customHeight="1" r="892" ht="15.0"/>
-    <row customHeight="1" r="893" ht="15.0"/>
-    <row customHeight="1" r="894" ht="15.0"/>
-    <row customHeight="1" r="895" ht="15.0"/>
-    <row customHeight="1" r="896" ht="15.0"/>
-    <row customHeight="1" r="897" ht="15.0"/>
-    <row customHeight="1" r="898" ht="15.0"/>
-    <row customHeight="1" r="899" ht="15.0"/>
-    <row customHeight="1" r="900" ht="15.0"/>
-    <row customHeight="1" r="901" ht="15.0"/>
-    <row customHeight="1" r="902" ht="15.0"/>
-    <row customHeight="1" r="903" ht="15.0"/>
-    <row customHeight="1" r="904" ht="15.0"/>
-    <row customHeight="1" r="905" ht="15.0"/>
-    <row customHeight="1" r="906" ht="15.0"/>
-    <row customHeight="1" r="907" ht="15.0"/>
-    <row customHeight="1" r="908" ht="15.0"/>
-    <row customHeight="1" r="909" ht="15.0"/>
-    <row customHeight="1" r="910" ht="15.0"/>
-    <row customHeight="1" r="911" ht="15.0"/>
-    <row customHeight="1" r="912" ht="15.0"/>
-    <row customHeight="1" r="913" ht="15.0"/>
-    <row customHeight="1" r="914" ht="15.0"/>
-    <row customHeight="1" r="915" ht="15.0"/>
-    <row customHeight="1" r="916" ht="15.0"/>
-    <row customHeight="1" r="917" ht="15.0"/>
-    <row customHeight="1" r="918" ht="15.0"/>
-    <row customHeight="1" r="919" ht="15.0"/>
-    <row customHeight="1" r="920" ht="15.0"/>
-    <row customHeight="1" r="921" ht="15.0"/>
-    <row customHeight="1" r="922" ht="15.0"/>
-    <row customHeight="1" r="923" ht="15.0"/>
-    <row customHeight="1" r="924" ht="15.0"/>
-    <row customHeight="1" r="925" ht="15.0"/>
-    <row customHeight="1" r="926" ht="15.0"/>
-    <row customHeight="1" r="927" ht="15.0"/>
-    <row customHeight="1" r="928" ht="15.0"/>
-    <row customHeight="1" r="929" ht="15.0"/>
-    <row customHeight="1" r="930" ht="15.0"/>
-    <row customHeight="1" r="931" ht="15.0"/>
-    <row customHeight="1" r="932" ht="15.0"/>
-    <row customHeight="1" r="933" ht="15.0"/>
-    <row customHeight="1" r="934" ht="15.0"/>
-    <row customHeight="1" r="935" ht="15.0"/>
-    <row customHeight="1" r="936" ht="15.0"/>
-    <row customHeight="1" r="937" ht="15.0"/>
-    <row customHeight="1" r="938" ht="15.0"/>
-    <row customHeight="1" r="939" ht="15.0"/>
-    <row customHeight="1" r="940" ht="15.0"/>
-    <row customHeight="1" r="941" ht="15.0"/>
-    <row customHeight="1" r="942" ht="15.0"/>
-    <row customHeight="1" r="943" ht="15.0"/>
-    <row customHeight="1" r="944" ht="15.0"/>
-    <row customHeight="1" r="945" ht="15.0"/>
-    <row customHeight="1" r="946" ht="15.0"/>
-    <row customHeight="1" r="947" ht="15.0"/>
-    <row customHeight="1" r="948" ht="15.0"/>
-    <row customHeight="1" r="949" ht="15.0"/>
-    <row customHeight="1" r="950" ht="15.0"/>
-    <row customHeight="1" r="951" ht="15.0"/>
-    <row customHeight="1" r="952" ht="15.0"/>
-    <row customHeight="1" r="953" ht="15.0"/>
-    <row customHeight="1" r="954" ht="15.0"/>
-    <row customHeight="1" r="955" ht="15.0"/>
-    <row customHeight="1" r="956" ht="15.0"/>
-    <row customHeight="1" r="957" ht="15.0"/>
-    <row customHeight="1" r="958" ht="15.0"/>
-    <row customHeight="1" r="959" ht="15.0"/>
-    <row customHeight="1" r="960" ht="15.0"/>
-    <row customHeight="1" r="961" ht="15.0"/>
-    <row customHeight="1" r="962" ht="15.0"/>
-    <row customHeight="1" r="963" ht="15.0"/>
-    <row customHeight="1" r="964" ht="15.0"/>
-    <row customHeight="1" r="965" ht="15.0"/>
-    <row customHeight="1" r="966" ht="15.0"/>
-    <row customHeight="1" r="967" ht="15.0"/>
-    <row customHeight="1" r="968" ht="15.0"/>
-    <row customHeight="1" r="969" ht="15.0"/>
-    <row customHeight="1" r="970" ht="15.0"/>
-    <row customHeight="1" r="971" ht="15.0"/>
-    <row customHeight="1" r="972" ht="15.0"/>
-    <row customHeight="1" r="973" ht="15.0"/>
-    <row customHeight="1" r="974" ht="15.0"/>
-    <row customHeight="1" r="975" ht="15.0"/>
-    <row customHeight="1" r="976" ht="15.0"/>
-    <row customHeight="1" r="977" ht="15.0"/>
-    <row customHeight="1" r="978" ht="15.0"/>
-    <row customHeight="1" r="979" ht="15.0"/>
-    <row customHeight="1" r="980" ht="15.0"/>
-    <row customHeight="1" r="981" ht="15.0"/>
-    <row customHeight="1" r="982" ht="15.0"/>
-    <row customHeight="1" r="983" ht="15.0"/>
-    <row customHeight="1" r="984" ht="15.0"/>
-    <row customHeight="1" r="985" ht="15.0"/>
-    <row customHeight="1" r="986" ht="15.0"/>
-    <row customHeight="1" r="987" ht="15.0"/>
-    <row customHeight="1" r="988" ht="15.0"/>
-    <row customHeight="1" r="989" ht="15.0"/>
-    <row customHeight="1" r="990" ht="15.0"/>
-    <row customHeight="1" r="991" ht="15.0"/>
-    <row customHeight="1" r="992" ht="15.0"/>
-    <row customHeight="1" r="993" ht="15.0"/>
-    <row customHeight="1" r="994" ht="15.0"/>
-    <row customHeight="1" r="995" ht="15.0"/>
-    <row customHeight="1" r="996" ht="15.0"/>
-    <row customHeight="1" r="997" ht="15.0"/>
-    <row customHeight="1" r="998" ht="15.0"/>
-    <row customHeight="1" r="999" ht="15.0"/>
-    <row customHeight="1" r="1000" ht="15.0"/>
-    <row customHeight="1" r="1001" ht="15.0"/>
-    <row customHeight="1" r="1002" ht="15.0"/>
-    <row customHeight="1" r="1003" ht="15.0"/>
-    <row customHeight="1" r="1004" ht="15.0"/>
-    <row customHeight="1" r="1005" ht="15.0"/>
-    <row customHeight="1" r="1006" ht="15.0"/>
-    <row customHeight="1" r="1007" ht="15.0"/>
-    <row customHeight="1" r="1008" ht="15.0"/>
-    <row customHeight="1" r="1009" ht="15.0"/>
-    <row customHeight="1" r="1010" ht="15.0"/>
-    <row customHeight="1" r="1011" ht="15.0"/>
-    <row customHeight="1" r="1012" ht="15.0"/>
-    <row customHeight="1" r="1013" ht="15.0"/>
-    <row customHeight="1" r="1014" ht="15.0"/>
-    <row customHeight="1" r="1015" ht="15.0"/>
-    <row customHeight="1" r="1016" ht="15.0"/>
-    <row customHeight="1" r="1017" ht="15.0"/>
-    <row customHeight="1" r="1018" ht="15.0"/>
-    <row customHeight="1" r="1019" ht="15.0"/>
-    <row customHeight="1" r="1020" ht="15.0"/>
-    <row customHeight="1" r="1021" ht="15.0"/>
-    <row customHeight="1" r="1022" ht="15.0"/>
-    <row customHeight="1" r="1023" ht="15.0"/>
-    <row customHeight="1" r="1024" ht="15.0"/>
-    <row customHeight="1" r="1025" ht="15.0"/>
-    <row customHeight="1" r="1026" ht="15.0"/>
-    <row customHeight="1" r="1027" ht="15.0"/>
-    <row customHeight="1" r="1028" ht="15.0"/>
-    <row customHeight="1" r="1029" ht="15.0"/>
-    <row customHeight="1" r="1030" ht="15.0"/>
-    <row customHeight="1" r="1031" ht="15.0"/>
-    <row customHeight="1" r="1032" ht="15.0"/>
-    <row customHeight="1" r="1033" ht="15.0"/>
-    <row customHeight="1" r="1034" ht="15.0"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A10"/>
@@ -5119,76 +3819,169 @@
       </c>
     </row>
     <row customHeight="1" r="18" ht="15.0">
-      <c t="s" s="5" r="B18">
+      <c s="4" r="B18">
+        <v>15.0</v>
+      </c>
+      <c s="4" r="C18">
+        <v>15.1</v>
+      </c>
+      <c s="4" r="D18">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="E18">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="F18">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="G18">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="H18">
+        <v>0.0</v>
+      </c>
+      <c s="4" r="I18">
+        <v>0.0</v>
+      </c>
+      <c s="4" r="J18">
+        <v>0.0</v>
+      </c>
+      <c s="4" r="K18">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row customHeight="1" r="19" ht="15.0">
+      <c s="4" r="B19">
+        <v>16.0</v>
+      </c>
+      <c s="4" r="C19">
+        <v>16.1</v>
+      </c>
+      <c s="4" r="D19">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="E19">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="F19">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="G19">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="H19">
+        <v>0.0</v>
+      </c>
+      <c s="4" r="I19">
+        <v>0.0</v>
+      </c>
+      <c s="4" r="J19">
+        <v>0.0</v>
+      </c>
+      <c s="4" r="K19">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row customHeight="1" r="20" ht="15.0">
+      <c s="4" r="B20">
+        <v>17.0</v>
+      </c>
+      <c s="4" r="C20">
+        <v>17.1</v>
+      </c>
+      <c s="4" r="D20">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="E20">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="F20">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="G20">
+        <v>1.0</v>
+      </c>
+      <c s="4" r="H20">
+        <v>0.0</v>
+      </c>
+      <c s="4" r="I20">
+        <v>0.0</v>
+      </c>
+      <c s="4" r="J20">
+        <v>0.0</v>
+      </c>
+      <c s="4" r="K20">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row customHeight="1" r="21" ht="15.0">
+      <c t="s" s="5" r="B21">
         <v>33</v>
       </c>
-      <c t="str" s="4" r="D18">
-        <f>SUM(D2:D17)</f>
-        <v>15</v>
-      </c>
-      <c s="1" r="E18">
+      <c t="str" s="4" r="D21">
+        <f>SUM(D2:D20)</f>
+        <v>18</v>
+      </c>
+      <c s="1" r="E21">
+        <v>15.43</v>
+      </c>
+      <c s="1" r="F21">
         <v>12.86</v>
       </c>
-      <c s="1" r="F18">
-        <v>10.72</v>
-      </c>
-      <c s="1" r="G18">
-        <v>8.58</v>
-      </c>
-      <c s="1" r="H18">
-        <v>6.44</v>
-      </c>
-      <c s="1" r="I18">
-        <v>4.3</v>
-      </c>
-      <c s="4" r="J18">
-        <v>2.16</v>
-      </c>
-      <c s="4" r="K18">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row customHeight="1" r="19" ht="15.0">
-      <c s="4" r="A19"/>
-      <c t="s" s="5" r="B19">
+      <c s="1" r="G21">
+        <v>10.29</v>
+      </c>
+      <c s="1" r="H21">
+        <v>7.72</v>
+      </c>
+      <c s="1" r="I21">
+        <v>5.15</v>
+      </c>
+      <c s="4" r="J21">
+        <v>2.58</v>
+      </c>
+      <c s="4" r="K21">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row customHeight="1" r="22" ht="15.0">
+      <c s="4" r="A22"/>
+      <c t="s" s="5" r="B22">
         <v>34</v>
       </c>
-      <c t="str" s="4" r="D19">
-        <f ref="D19:K19" t="shared" si="1">SUM(D2:D17)</f>
-        <v>15</v>
-      </c>
-      <c t="str" s="4" r="E19">
+      <c t="str" s="4" r="D22">
+        <f ref="D22:K22" t="shared" si="1">SUM(D2:D20)</f>
+        <v>18</v>
+      </c>
+      <c t="str" s="4" r="E22">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c t="str" s="4" r="F19">
+        <v>17</v>
+      </c>
+      <c t="str" s="4" r="F22">
         <f t="shared" si="1"/>
-        <v>13.5</v>
-      </c>
-      <c t="str" s="4" r="G19">
+        <v>16.5</v>
+      </c>
+      <c t="str" s="4" r="G22">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c t="str" s="4" r="H19">
+        <v>16</v>
+      </c>
+      <c t="str" s="4" r="H22">
         <f t="shared" si="1"/>
         <v>11.5</v>
       </c>
-      <c t="str" s="4" r="I19">
+      <c t="str" s="4" r="I22">
         <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
-      <c t="str" s="4" r="J19">
+      <c t="str" s="4" r="J22">
         <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
-      <c t="str" s="4" r="K19">
+      <c t="str" s="4" r="K22">
         <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
     </row>
-    <row customHeight="1" r="20" ht="15.0"/>
-    <row customHeight="1" r="21" ht="15.0"/>
-    <row customHeight="1" r="22" ht="15.0"/>
     <row customHeight="1" r="23" ht="15.0"/>
     <row customHeight="1" r="24" ht="15.0"/>
     <row customHeight="1" r="25" ht="15.0"/>
@@ -5209,11 +4002,14 @@
     <row customHeight="1" r="40" ht="15.0"/>
     <row customHeight="1" r="41" ht="15.0"/>
     <row customHeight="1" r="42" ht="15.0"/>
+    <row customHeight="1" r="43" ht="15.0"/>
+    <row customHeight="1" r="44" ht="15.0"/>
+    <row customHeight="1" r="45" ht="15.0"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A2:A21"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update week 8 iteration. Finish week 8 burndown chart.
</commit_message>
<xml_diff>
--- a/Project Management/Iteration Planning/Burndown_Charts.xlsx
+++ b/Project Management/Iteration Planning/Burndown_Charts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" firstSheet="1" activeTab="7"/>
@@ -208,8 +208,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -236,6 +238,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -243,14 +251,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -261,6 +263,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -271,6 +274,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -301,7 +305,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -416,11 +419,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2047388424"/>
-        <c:axId val="2081545976"/>
+        <c:axId val="2106687560"/>
+        <c:axId val="2107879992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2047388424"/>
+        <c:axId val="2106687560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -442,7 +445,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="cross"/>
@@ -458,7 +460,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081545976"/>
+        <c:crossAx val="2107879992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -466,7 +468,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081545976"/>
+        <c:axId val="2107879992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -497,7 +499,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -519,14 +520,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2047388424"/>
+        <c:crossAx val="2106687560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -564,7 +564,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -679,11 +678,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2083111848"/>
-        <c:axId val="2083117064"/>
+        <c:axId val="2106635432"/>
+        <c:axId val="2106630088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2083111848"/>
+        <c:axId val="2106635432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,7 +704,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="cross"/>
@@ -721,7 +719,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083117064"/>
+        <c:crossAx val="2106630088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -729,7 +727,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083117064"/>
+        <c:axId val="2106630088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -760,7 +758,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -782,14 +779,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083111848"/>
+        <c:crossAx val="2106635432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -827,7 +823,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -942,11 +937,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081497736"/>
-        <c:axId val="2081492472"/>
+        <c:axId val="2063560008"/>
+        <c:axId val="2063565336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081497736"/>
+        <c:axId val="2063560008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,7 +963,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="cross"/>
@@ -984,7 +978,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081492472"/>
+        <c:crossAx val="2063565336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -992,7 +986,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081492472"/>
+        <c:axId val="2063565336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1023,7 +1017,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1045,14 +1038,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081497736"/>
+        <c:crossAx val="2063560008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1090,7 +1082,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1205,11 +1196,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081438648"/>
-        <c:axId val="2081433400"/>
+        <c:axId val="2109224040"/>
+        <c:axId val="2109229368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081438648"/>
+        <c:axId val="2109224040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1222,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="cross"/>
@@ -1247,7 +1237,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081433400"/>
+        <c:crossAx val="2109229368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1255,7 +1245,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081433400"/>
+        <c:axId val="2109229368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1276,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1308,14 +1297,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081438648"/>
+        <c:crossAx val="2109224040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1449,11 +1437,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2084055080"/>
-        <c:axId val="2084057960"/>
+        <c:axId val="2109261112"/>
+        <c:axId val="2109263992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2084055080"/>
+        <c:axId val="2109261112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084057960"/>
+        <c:crossAx val="2109263992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1481,7 +1469,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2084057960"/>
+        <c:axId val="2109263992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1515,14 +1503,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084055080"/>
+        <c:crossAx val="2109261112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1567,7 +1554,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1690,11 +1676,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2097321192"/>
-        <c:axId val="2097322600"/>
+        <c:axId val="2109278696"/>
+        <c:axId val="2109284152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2097321192"/>
+        <c:axId val="2109278696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1716,13 +1702,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097322600"/>
+        <c:crossAx val="2109284152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1730,7 +1715,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097322600"/>
+        <c:axId val="2109284152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1753,21 +1738,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097321192"/>
+        <c:crossAx val="2109278696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1935,11 +1918,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2097343096"/>
-        <c:axId val="2097345832"/>
+        <c:axId val="2065434392"/>
+        <c:axId val="2065439864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2097343096"/>
+        <c:axId val="2065434392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1967,7 +1950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097345832"/>
+        <c:crossAx val="2065439864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1975,7 +1958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097345832"/>
+        <c:axId val="2065439864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2005,7 +1988,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097343096"/>
+        <c:crossAx val="2065434392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2146,6 +2129,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2161,11 +2168,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2088764424"/>
-        <c:axId val="2088898680"/>
+        <c:axId val="2107831096"/>
+        <c:axId val="2107825608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2088764424"/>
+        <c:axId val="2107831096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,7 +2200,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088898680"/>
+        <c:crossAx val="2107825608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2201,7 +2208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2088898680"/>
+        <c:axId val="2107825608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2231,7 +2238,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088764424"/>
+        <c:crossAx val="2107831096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2851,7 +2858,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
@@ -2886,7 +2893,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="A3" s="5"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1">
         <v>5</v>
       </c>
@@ -2919,7 +2926,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="5"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1">
         <v>5</v>
       </c>
@@ -2952,7 +2959,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
-      <c r="A5" s="5"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1">
         <v>5</v>
       </c>
@@ -2985,7 +2992,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
-      <c r="A6" s="5"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1">
         <v>5</v>
       </c>
@@ -3018,7 +3025,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
-      <c r="A7" s="5"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -3051,7 +3058,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="A8" s="5"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -3084,7 +3091,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -3117,11 +3124,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="1">
         <f>SUM(D2:D9)</f>
         <v>5</v>
@@ -3150,10 +3157,10 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="1">
         <f t="shared" ref="D11:I11" si="0">SUM(D2:D9)</f>
         <v>5</v>
@@ -3289,7 +3296,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1">
@@ -3324,7 +3331,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="A3" s="5"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1">
         <v>6</v>
       </c>
@@ -3357,7 +3364,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="5"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1">
         <v>8</v>
       </c>
@@ -3390,7 +3397,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
-      <c r="A5" s="5"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1">
         <v>8</v>
       </c>
@@ -3423,7 +3430,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
-      <c r="A6" s="5"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1">
         <v>13</v>
       </c>
@@ -3456,7 +3463,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
-      <c r="A7" s="5"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1">
         <v>7</v>
       </c>
@@ -3489,11 +3496,11 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="1">
         <f>SUM(D2:D7)</f>
         <v>8</v>
@@ -3521,11 +3528,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="1">
         <f t="shared" ref="D9:K9" si="0">SUM(D2:D7)</f>
         <v>8</v>
@@ -3560,7 +3567,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="5"/>
+      <c r="A10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1"/>
     <row r="12" spans="1:11" ht="15" customHeight="1"/>
@@ -3646,7 +3653,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="1">
@@ -3681,7 +3688,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="A3" s="5"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1">
         <v>8</v>
       </c>
@@ -3714,7 +3721,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="5"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1">
         <v>13</v>
       </c>
@@ -3747,7 +3754,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
-      <c r="A5" s="5"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1">
         <v>9</v>
       </c>
@@ -3780,7 +3787,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
-      <c r="A6" s="5"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1">
         <v>9</v>
       </c>
@@ -3813,7 +3820,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
-      <c r="A7" s="5"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1">
         <v>9</v>
       </c>
@@ -3846,7 +3853,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="A8" s="5"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1">
         <v>9</v>
       </c>
@@ -3879,7 +3886,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="1">
         <v>9</v>
       </c>
@@ -3912,7 +3919,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="5"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="1">
         <v>9</v>
       </c>
@@ -3945,7 +3952,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
-      <c r="A11" s="5"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1">
         <v>10</v>
       </c>
@@ -3978,7 +3985,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
-      <c r="A12" s="5"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -4011,7 +4018,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
-      <c r="A13" s="5"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1">
         <v>10</v>
       </c>
@@ -4044,11 +4051,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="1">
         <f>SUM(D2:D13)</f>
         <v>12</v>
@@ -4076,10 +4083,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="1">
         <f t="shared" ref="D15:K15" si="0">SUM(D2:D13)</f>
         <v>12</v>
@@ -4201,7 +4208,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="3">
@@ -4236,7 +4243,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="A3" s="5"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="3">
         <v>13</v>
       </c>
@@ -4269,7 +4276,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="5"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="3">
         <v>9</v>
       </c>
@@ -4302,7 +4309,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
-      <c r="A5" s="5"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="3">
         <v>9</v>
       </c>
@@ -4335,7 +4342,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
-      <c r="A6" s="5"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="3">
         <v>9</v>
       </c>
@@ -4368,7 +4375,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
-      <c r="A7" s="5"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="3">
         <v>9</v>
       </c>
@@ -4401,7 +4408,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="A8" s="5"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="3">
         <v>10</v>
       </c>
@@ -4434,7 +4441,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="3">
         <v>10</v>
       </c>
@@ -4467,7 +4474,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="5"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="3">
         <v>3</v>
       </c>
@@ -4500,7 +4507,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
-      <c r="A11" s="5"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="3">
         <v>3</v>
       </c>
@@ -4533,7 +4540,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
-      <c r="A12" s="5"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="3">
         <v>4</v>
       </c>
@@ -4566,7 +4573,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
-      <c r="A13" s="5"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="3">
         <v>4</v>
       </c>
@@ -4599,7 +4606,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="3">
         <v>4</v>
       </c>
@@ -4632,7 +4639,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="A15" s="5"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="3">
         <v>4</v>
       </c>
@@ -4665,7 +4672,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="A16" s="5"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="3">
         <v>11</v>
       </c>
@@ -4698,7 +4705,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
-      <c r="A17" s="5"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="3">
         <v>11</v>
       </c>
@@ -4731,7 +4738,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1">
-      <c r="A18" s="5"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="3">
         <v>11</v>
       </c>
@@ -4764,11 +4771,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="3">
         <f>SUM(D2:D18)</f>
         <v>16</v>
@@ -4797,10 +4804,10 @@
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1">
       <c r="A20" s="3"/>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="3">
         <f t="shared" ref="D20:K20" si="0">SUM(D2:D18)</f>
         <v>16</v>
@@ -4922,7 +4929,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="3">
@@ -4957,7 +4964,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="A3" s="5"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="3">
         <v>9</v>
       </c>
@@ -4990,7 +4997,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="5"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="3">
         <v>9</v>
       </c>
@@ -5023,7 +5030,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
-      <c r="A5" s="5"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="3">
         <v>10</v>
       </c>
@@ -5056,7 +5063,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
-      <c r="A6" s="5"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="3">
         <v>10</v>
       </c>
@@ -5089,7 +5096,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
-      <c r="A7" s="5"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="3">
         <v>3</v>
       </c>
@@ -5122,7 +5129,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="A8" s="5"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="3">
         <v>3</v>
       </c>
@@ -5155,7 +5162,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="3">
         <v>4</v>
       </c>
@@ -5188,7 +5195,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="5"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="3">
         <v>4</v>
       </c>
@@ -5221,7 +5228,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
-      <c r="A11" s="5"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="3">
         <v>4</v>
       </c>
@@ -5254,7 +5261,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
-      <c r="A12" s="5"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="3">
         <v>4</v>
       </c>
@@ -5287,7 +5294,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
-      <c r="A13" s="5"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="3">
         <v>11</v>
       </c>
@@ -5320,7 +5327,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="3">
         <v>11</v>
       </c>
@@ -5353,7 +5360,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="A15" s="5"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="3">
         <v>11</v>
       </c>
@@ -5386,7 +5393,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="A16" s="5"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="3">
         <v>14</v>
       </c>
@@ -5419,7 +5426,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
-      <c r="A17" s="5"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="3">
         <v>14</v>
       </c>
@@ -5452,7 +5459,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1">
-      <c r="A18" s="5"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="3">
         <v>15</v>
       </c>
@@ -5485,7 +5492,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1">
-      <c r="A19" s="5"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="3">
         <v>16</v>
       </c>
@@ -5518,7 +5525,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1">
-      <c r="A20" s="5"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="3">
         <v>17</v>
       </c>
@@ -5551,11 +5558,11 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="3">
         <f>SUM(D2:D20)</f>
         <v>18</v>
@@ -5584,10 +5591,10 @@
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1">
       <c r="A22" s="3"/>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="3">
         <f t="shared" ref="D22:K22" si="0">SUM(D2:D20)</f>
         <v>18</v>
@@ -5709,7 +5716,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="3">
@@ -5744,7 +5751,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="A3" s="5"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="3">
         <v>9</v>
       </c>
@@ -5777,7 +5784,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="5"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="3">
         <v>10</v>
       </c>
@@ -5810,7 +5817,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
-      <c r="A5" s="5"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="3">
         <v>10</v>
       </c>
@@ -5843,7 +5850,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
-      <c r="A6" s="5"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -5876,7 +5883,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
-      <c r="A7" s="5"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="3">
         <v>11</v>
       </c>
@@ -5909,7 +5916,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="A8" s="5"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="3">
         <v>11</v>
       </c>
@@ -5942,7 +5949,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="3">
         <v>14</v>
       </c>
@@ -5975,7 +5982,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="5"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="3">
         <v>12</v>
       </c>
@@ -6008,7 +6015,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
-      <c r="A11" s="5"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="3">
         <v>12</v>
       </c>
@@ -6041,7 +6048,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
-      <c r="A12" s="5"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="3">
         <v>12</v>
       </c>
@@ -6074,7 +6081,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
-      <c r="A13" s="5"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="3">
         <v>20</v>
       </c>
@@ -6107,7 +6114,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="3">
         <v>20</v>
       </c>
@@ -6140,7 +6147,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="A15" s="5"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="3">
         <v>20</v>
       </c>
@@ -6173,7 +6180,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="A16" s="5"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="3">
         <v>20</v>
       </c>
@@ -6206,7 +6213,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
-      <c r="A17" s="5"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="3">
         <v>21</v>
       </c>
@@ -6239,7 +6246,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1">
-      <c r="A18" s="5"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="3">
         <v>21</v>
       </c>
@@ -6272,7 +6279,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1">
-      <c r="A19" s="5"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="3">
         <v>22</v>
       </c>
@@ -6305,7 +6312,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1">
-      <c r="A20" s="5"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="3">
         <v>22</v>
       </c>
@@ -6338,8 +6345,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="C21" s="7" t="s">
+      <c r="A21" s="9"/>
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="3">
@@ -6370,7 +6377,7 @@
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1">
       <c r="A22" s="3"/>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="3">
@@ -6492,7 +6499,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3">
@@ -6527,7 +6534,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15">
-      <c r="A3" s="4"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="3">
         <v>12</v>
       </c>
@@ -6560,7 +6567,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15">
-      <c r="A4" s="4"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="3">
         <v>12</v>
       </c>
@@ -6593,7 +6600,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15">
-      <c r="A5" s="4"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="3">
         <v>21</v>
       </c>
@@ -6626,7 +6633,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15">
-      <c r="A6" s="4"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3">
         <v>21</v>
       </c>
@@ -6659,7 +6666,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15">
-      <c r="A7" s="4"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="3">
         <v>21</v>
       </c>
@@ -6692,7 +6699,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15">
-      <c r="A8" s="4"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3">
         <v>18</v>
       </c>
@@ -6725,7 +6732,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15">
-      <c r="A9" s="4"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3">
         <v>18</v>
       </c>
@@ -6758,7 +6765,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15">
-      <c r="A10" s="4"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="3">
         <v>18</v>
       </c>
@@ -6791,7 +6798,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15">
-      <c r="A11" s="4"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="3">
         <v>18</v>
       </c>
@@ -6824,7 +6831,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15">
-      <c r="A12" s="4"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
@@ -6857,7 +6864,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15">
-      <c r="A13" s="4"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="3" t="s">
         <v>42</v>
       </c>
@@ -6890,7 +6897,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15">
-      <c r="A14" s="4"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="3" t="s">
         <v>42</v>
       </c>
@@ -6923,7 +6930,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15">
-      <c r="A15" s="4"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="3" t="s">
         <v>42</v>
       </c>
@@ -6956,9 +6963,9 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15">
-      <c r="A16" s="4"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="3">
@@ -6988,55 +6995,55 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15">
-      <c r="A17" s="4"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="3">
-        <f>SUM(D2:D15)</f>
+        <f t="shared" ref="D17:K17" si="0">SUM(D2:D15)</f>
         <v>15.25</v>
       </c>
       <c r="E17" s="3">
-        <f>SUM(E2:E15)</f>
+        <f t="shared" si="0"/>
         <v>14.75</v>
       </c>
       <c r="F17" s="3">
-        <f>SUM(F2:F15)</f>
+        <f t="shared" si="0"/>
         <v>14.25</v>
       </c>
       <c r="G17" s="3">
-        <f>SUM(G2:G15)</f>
+        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
       <c r="H17" s="3">
-        <f>SUM(H2:H15)</f>
+        <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
       <c r="I17" s="3">
-        <f>SUM(I2:I15)</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="J17" s="3">
-        <f>SUM(J2:J15)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K17" s="3">
-        <f>SUM(K2:K15)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="8"/>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="8"/>
+      <c r="A19" s="5"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="8"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="8"/>
+      <c r="A21" s="5"/>
     </row>
     <row r="22" spans="1:11" ht="15">
       <c r="A22" s="3"/>
@@ -7060,8 +7067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -7080,29 +7087,29 @@
         <v>3</v>
       </c>
       <c r="E1" s="2">
-        <v>41957</v>
+        <v>41964</v>
       </c>
       <c r="F1" s="2">
-        <v>41958</v>
+        <v>41965</v>
       </c>
       <c r="G1" s="2">
-        <v>41959</v>
+        <v>41966</v>
       </c>
       <c r="H1" s="2">
-        <v>41960</v>
+        <v>41967</v>
       </c>
       <c r="I1" s="2">
-        <v>41961</v>
+        <v>41968</v>
       </c>
       <c r="J1" s="2">
-        <v>41962</v>
+        <v>41969</v>
       </c>
       <c r="K1" s="2">
-        <v>41963</v>
+        <v>41970</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3">
@@ -7114,16 +7121,30 @@
       <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="15">
-      <c r="A3" s="4"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="3">
         <v>18</v>
       </c>
@@ -7133,16 +7154,30 @@
       <c r="D3" s="3">
         <v>1.5</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="E3" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="15">
-      <c r="A4" s="4"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="3">
         <v>23</v>
       </c>
@@ -7152,16 +7187,30 @@
       <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="15">
-      <c r="A5" s="4"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -7171,16 +7220,30 @@
       <c r="D5" s="3">
         <v>0.5</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="E5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15">
-      <c r="A6" s="4"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3">
         <v>2</v>
       </c>
@@ -7190,16 +7253,30 @@
       <c r="D6" s="3">
         <v>0.5</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="E6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="15">
-      <c r="A7" s="4"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="3">
         <v>2</v>
       </c>
@@ -7209,16 +7286,30 @@
       <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15">
-      <c r="A8" s="4"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3">
         <v>19</v>
       </c>
@@ -7228,16 +7319,30 @@
       <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="15">
-      <c r="A9" s="4"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3">
         <v>19</v>
       </c>
@@ -7247,53 +7352,130 @@
       <c r="D9" s="3">
         <v>1</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15">
-      <c r="A10" s="4"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="10">
-        <v>2</v>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15">
-      <c r="A11" s="4"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="10">
-        <v>2</v>
-      </c>
-      <c r="D11" s="10">
-        <v>2</v>
+      <c r="C11" s="7">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>2</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>3</v>
       </c>
-      <c r="D12" s="10">
-        <v>2</v>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15">
-      <c r="A13" s="9"/>
-      <c r="C13" s="7" t="s">
+      <c r="A13" s="6"/>
+      <c r="C13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="3">
@@ -7323,27 +7505,51 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15">
-      <c r="A14" s="9"/>
-      <c r="C14" s="7" t="s">
+      <c r="A14" s="6"/>
+      <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="D14" s="3">
+        <f>SUM(D2:D12)</f>
+        <v>14.5</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" ref="E14:K14" si="0">SUM(E2:E12)</f>
+        <v>14.5</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>14.5</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="15">
-      <c r="A15" s="9"/>
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:11" ht="12" customHeight="1">
-      <c r="A16" s="9"/>
+      <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:1" ht="12" customHeight="1">
-      <c r="A17" s="9"/>
+      <c r="A17" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>